<commit_message>
actualizacion 05 junio de 2016
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -379,7 +379,7 @@
         <v>34</v>
       </c>
       <c r="B1" t="str">
-        <v>2016-05-16T19:02:53+02:00</v>
+        <v>19:02:53</v>
       </c>
     </row>
     <row r="2">
@@ -387,7 +387,7 @@
         <v>36</v>
       </c>
       <c r="B2" t="str">
-        <v>2016-05-16T19:00:25+02:00</v>
+        <v>19:00:25</v>
       </c>
     </row>
     <row r="3">
@@ -395,7 +395,7 @@
         <v>43</v>
       </c>
       <c r="B3" t="str">
-        <v>2016-05-16T19:01:05+02:00</v>
+        <v>19:01:05</v>
       </c>
     </row>
     <row r="4">
@@ -403,7 +403,7 @@
         <v>38</v>
       </c>
       <c r="B4" t="str">
-        <v>2016-05-16T19:01:13+02:00</v>
+        <v>19:01:13</v>
       </c>
     </row>
     <row r="5">
@@ -411,7 +411,7 @@
         <v>45</v>
       </c>
       <c r="B5" t="str">
-        <v>2016-05-16T18:59:37+02:00</v>
+        <v>18:59:37</v>
       </c>
     </row>
     <row r="6">
@@ -419,7 +419,7 @@
         <v>42</v>
       </c>
       <c r="B6" t="str">
-        <v>2016-05-16T19:01:25+02:00</v>
+        <v>19:01:25</v>
       </c>
     </row>
     <row r="7">
@@ -427,7 +427,7 @@
         <v>38</v>
       </c>
       <c r="B7" t="str">
-        <v>2016-05-16T19:01:53+02:00</v>
+        <v>19:01:53</v>
       </c>
     </row>
     <row r="8">
@@ -435,7 +435,7 @@
         <v>38</v>
       </c>
       <c r="B8" t="str">
-        <v>2016-05-16T19:00:01+02:00</v>
+        <v>19:00:01</v>
       </c>
     </row>
     <row r="9">
@@ -443,7 +443,7 @@
         <v>47</v>
       </c>
       <c r="B9" t="str">
-        <v>2016-05-16T19:00:29+02:00</v>
+        <v>19:00:29</v>
       </c>
     </row>
     <row r="10">
@@ -451,7 +451,7 @@
         <v>40</v>
       </c>
       <c r="B10" t="str">
-        <v>2016-05-16T19:00:33+02:00</v>
+        <v>19:00:33</v>
       </c>
     </row>
     <row r="11">
@@ -459,7 +459,7 @@
         <v>41</v>
       </c>
       <c r="B11" t="str">
-        <v>2016-05-16T19:02:33+02:00</v>
+        <v>19:02:33</v>
       </c>
     </row>
     <row r="12">
@@ -467,7 +467,7 @@
         <v>48</v>
       </c>
       <c r="B12" t="str">
-        <v>2016-05-16T19:02:49+02:00</v>
+        <v>19:02:49</v>
       </c>
     </row>
     <row r="13">
@@ -475,7 +475,7 @@
         <v>44</v>
       </c>
       <c r="B13" t="str">
-        <v>2016-05-16T19:01:33+02:00</v>
+        <v>19:01:33</v>
       </c>
     </row>
     <row r="14">
@@ -483,7 +483,7 @@
         <v>47</v>
       </c>
       <c r="B14" t="str">
-        <v>2016-05-16T19:02:29+02:00</v>
+        <v>19:02:29</v>
       </c>
     </row>
     <row r="15">
@@ -491,7 +491,7 @@
         <v>48</v>
       </c>
       <c r="B15" t="str">
-        <v>2016-05-16T19:01:21+02:00</v>
+        <v>19:01:21</v>
       </c>
     </row>
     <row r="16">
@@ -499,7 +499,7 @@
         <v>48</v>
       </c>
       <c r="B16" t="str">
-        <v>2016-05-16T19:01:37+02:00</v>
+        <v>19:01:37</v>
       </c>
     </row>
     <row r="17">
@@ -507,7 +507,7 @@
         <v>37</v>
       </c>
       <c r="B17" t="str">
-        <v>2016-05-16T19:02:41+02:00</v>
+        <v>19:02:41</v>
       </c>
     </row>
     <row r="18">
@@ -515,7 +515,7 @@
         <v>44</v>
       </c>
       <c r="B18" t="str">
-        <v>2016-05-16T19:03:13+02:00</v>
+        <v>19:03:13</v>
       </c>
     </row>
     <row r="19">
@@ -523,7 +523,7 @@
         <v>46</v>
       </c>
       <c r="B19" t="str">
-        <v>2016-05-16T19:00:41+02:00</v>
+        <v>19:00:41</v>
       </c>
     </row>
     <row r="20">
@@ -531,7 +531,7 @@
         <v>47</v>
       </c>
       <c r="B20" t="str">
-        <v>2016-05-16T19:02:17+02:00</v>
+        <v>19:02:17</v>
       </c>
     </row>
     <row r="21">
@@ -539,7 +539,7 @@
         <v>37</v>
       </c>
       <c r="B21" t="str">
-        <v>2016-05-16T19:02:13+02:00</v>
+        <v>19:02:13</v>
       </c>
     </row>
     <row r="22">
@@ -547,7 +547,7 @@
         <v>39</v>
       </c>
       <c r="B22" t="str">
-        <v>2016-05-16T19:00:09+02:00</v>
+        <v>19:00:09</v>
       </c>
     </row>
     <row r="23">
@@ -555,7 +555,7 @@
         <v>35</v>
       </c>
       <c r="B23" t="str">
-        <v>2016-05-16T19:03:25+02:00</v>
+        <v>19:03:25</v>
       </c>
     </row>
     <row r="24">
@@ -563,7 +563,7 @@
         <v>35</v>
       </c>
       <c r="B24" t="str">
-        <v>2016-05-16T19:02:57+02:00</v>
+        <v>19:02:57</v>
       </c>
     </row>
     <row r="25">
@@ -571,7 +571,7 @@
         <v>36</v>
       </c>
       <c r="B25" t="str">
-        <v>2016-05-16T19:01:57+02:00</v>
+        <v>19:01:57</v>
       </c>
     </row>
     <row r="26">
@@ -579,7 +579,7 @@
         <v>34</v>
       </c>
       <c r="B26" t="str">
-        <v>2016-05-16T19:01:09+02:00</v>
+        <v>19:01:09</v>
       </c>
     </row>
     <row r="27">
@@ -587,7 +587,7 @@
         <v>41</v>
       </c>
       <c r="B27" t="str">
-        <v>2016-05-16T19:00:21+02:00</v>
+        <v>19:00:21</v>
       </c>
     </row>
     <row r="28">
@@ -595,7 +595,7 @@
         <v>33</v>
       </c>
       <c r="B28" t="str">
-        <v>2016-05-16T19:00:57+02:00</v>
+        <v>19:00:57</v>
       </c>
     </row>
     <row r="29">
@@ -603,7 +603,7 @@
         <v>41</v>
       </c>
       <c r="B29" t="str">
-        <v>2016-05-16T19:00:05+02:00</v>
+        <v>19:00:05</v>
       </c>
     </row>
     <row r="30">
@@ -611,7 +611,7 @@
         <v>37</v>
       </c>
       <c r="B30" t="str">
-        <v>2016-05-16T19:03:21+02:00</v>
+        <v>19:03:21</v>
       </c>
     </row>
     <row r="31">
@@ -619,7 +619,7 @@
         <v>39</v>
       </c>
       <c r="B31" t="str">
-        <v>2016-05-16T19:02:01+02:00</v>
+        <v>19:02:01</v>
       </c>
     </row>
     <row r="32">
@@ -627,7 +627,7 @@
         <v>49</v>
       </c>
       <c r="B32" t="str">
-        <v>2016-05-16T18:59:53+02:00</v>
+        <v>18:59:53</v>
       </c>
     </row>
     <row r="33">
@@ -635,7 +635,7 @@
         <v>49</v>
       </c>
       <c r="B33" t="str">
-        <v>2016-05-16T19:01:17+02:00</v>
+        <v>19:01:17</v>
       </c>
     </row>
     <row r="34">
@@ -643,7 +643,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="str">
-        <v>2016-05-16T19:03:09+02:00</v>
+        <v>19:03:09</v>
       </c>
     </row>
     <row r="35">
@@ -651,7 +651,7 @@
         <v>39</v>
       </c>
       <c r="B35" t="str">
-        <v>2016-05-16T19:00:37+02:00</v>
+        <v>19:00:37</v>
       </c>
     </row>
     <row r="36">
@@ -659,7 +659,7 @@
         <v>40</v>
       </c>
       <c r="B36" t="str">
-        <v>2016-05-16T19:00:45+02:00</v>
+        <v>19:00:45</v>
       </c>
     </row>
     <row r="37">
@@ -667,7 +667,7 @@
         <v>43</v>
       </c>
       <c r="B37" t="str">
-        <v>2016-05-16T19:03:01+02:00</v>
+        <v>19:03:01</v>
       </c>
     </row>
     <row r="38">
@@ -675,7 +675,7 @@
         <v>33</v>
       </c>
       <c r="B38" t="str">
-        <v>2016-05-16T19:01:01+02:00</v>
+        <v>19:01:01</v>
       </c>
     </row>
     <row r="39">
@@ -683,7 +683,7 @@
         <v>43</v>
       </c>
       <c r="B39" t="str">
-        <v>2016-05-16T19:02:25+02:00</v>
+        <v>19:02:25</v>
       </c>
     </row>
     <row r="40">
@@ -691,7 +691,7 @@
         <v>32</v>
       </c>
       <c r="B40" t="str">
-        <v>2016-05-16T18:59:57+02:00</v>
+        <v>18:59:57</v>
       </c>
     </row>
     <row r="41">
@@ -699,7 +699,7 @@
         <v>47</v>
       </c>
       <c r="B41" t="str">
-        <v>2016-05-16T19:00:17+02:00</v>
+        <v>19:00:17</v>
       </c>
     </row>
     <row r="42">
@@ -707,7 +707,7 @@
         <v>36</v>
       </c>
       <c r="B42" t="str">
-        <v>2016-05-16T18:59:45+02:00</v>
+        <v>18:59:45</v>
       </c>
     </row>
     <row r="43">
@@ -715,7 +715,7 @@
         <v>38</v>
       </c>
       <c r="B43" t="str">
-        <v>2016-05-16T19:02:45+02:00</v>
+        <v>19:02:45</v>
       </c>
     </row>
     <row r="44">
@@ -723,7 +723,7 @@
         <v>49</v>
       </c>
       <c r="B44" t="str">
-        <v>2016-05-16T19:01:45+02:00</v>
+        <v>19:01:45</v>
       </c>
     </row>
     <row r="45">
@@ -731,7 +731,7 @@
         <v>47</v>
       </c>
       <c r="B45" t="str">
-        <v>2016-05-16T19:02:05+02:00</v>
+        <v>19:02:05</v>
       </c>
     </row>
     <row r="46">
@@ -739,7 +739,7 @@
         <v>37</v>
       </c>
       <c r="B46" t="str">
-        <v>2016-05-16T19:02:09+02:00</v>
+        <v>19:02:09</v>
       </c>
     </row>
     <row r="47">
@@ -747,7 +747,7 @@
         <v>38</v>
       </c>
       <c r="B47" t="str">
-        <v>2016-05-16T18:59:49+02:00</v>
+        <v>18:59:49</v>
       </c>
     </row>
     <row r="48">
@@ -755,7 +755,7 @@
         <v>37</v>
       </c>
       <c r="B48" t="str">
-        <v>2016-05-16T18:59:41+02:00</v>
+        <v>18:59:41</v>
       </c>
     </row>
     <row r="49">
@@ -763,7 +763,7 @@
         <v>44</v>
       </c>
       <c r="B49" t="str">
-        <v>2016-05-16T19:01:29+02:00</v>
+        <v>19:01:29</v>
       </c>
     </row>
     <row r="50">
@@ -771,7 +771,7 @@
         <v>48</v>
       </c>
       <c r="B50" t="str">
-        <v>2016-05-16T19:00:13+02:00</v>
+        <v>19:00:13</v>
       </c>
     </row>
     <row r="51">
@@ -779,7 +779,7 @@
         <v>41</v>
       </c>
       <c r="B51" t="str">
-        <v>2016-05-16T19:00:53+02:00</v>
+        <v>19:00:53</v>
       </c>
     </row>
     <row r="52">
@@ -787,7 +787,7 @@
         <v>44</v>
       </c>
       <c r="B52" t="str">
-        <v>2016-05-16T19:02:37+02:00</v>
+        <v>19:02:37</v>
       </c>
     </row>
     <row r="53">
@@ -795,7 +795,7 @@
         <v>43</v>
       </c>
       <c r="B53" t="str">
-        <v>2016-05-16T19:03:05+02:00</v>
+        <v>19:03:05</v>
       </c>
     </row>
     <row r="54">
@@ -803,7 +803,7 @@
         <v>41</v>
       </c>
       <c r="B54" t="str">
-        <v>2016-05-16T19:01:49+02:00</v>
+        <v>19:01:49</v>
       </c>
     </row>
     <row r="55">
@@ -811,7 +811,7 @@
         <v>37</v>
       </c>
       <c r="B55" t="str">
-        <v>2016-05-16T19:03:17+02:00</v>
+        <v>19:03:17</v>
       </c>
     </row>
     <row r="56">
@@ -819,7 +819,7 @@
         <v>41</v>
       </c>
       <c r="B56" t="str">
-        <v>2016-05-16T19:01:41+02:00</v>
+        <v>19:01:41</v>
       </c>
     </row>
     <row r="57">
@@ -827,7 +827,7 @@
         <v>33</v>
       </c>
       <c r="B57" t="str">
-        <v>2016-05-16T19:00:49+02:00</v>
+        <v>19:00:49</v>
       </c>
     </row>
     <row r="58">
@@ -835,7 +835,7 @@
         <v>41</v>
       </c>
       <c r="B58" t="str">
-        <v>2016-05-16T19:02:21+02:00</v>
+        <v>19:02:21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>